<commit_message>
[assessment] update after 18.10.2018
</commit_message>
<xml_diff>
--- a/obecnosci_i_oceny.xlsx
+++ b/obecnosci_i_oceny.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neegra/paradygmaty-programowania/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E1DE5B-F6C5-8A4E-B143-0FAF7F950CCB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA43A5F-98FB-AF47-80F4-14EA97676B25}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="17100" xr2:uid="{97166A3A-37EA-D446-B119-A32076EDFA0A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>ALBUM</t>
   </si>
@@ -139,13 +139,28 @@
   </si>
   <si>
     <t>2.0</t>
+  </si>
+  <si>
+    <t>LEGENDA</t>
+  </si>
+  <si>
+    <t>nieobecność</t>
+  </si>
+  <si>
+    <t>nieobecność usprawiedliwiona</t>
+  </si>
+  <si>
+    <t>obecność</t>
+  </si>
+  <si>
+    <t>obecność bez wysłanej listy po laboratoriach</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -168,8 +183,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="6"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -194,8 +225,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -403,11 +446,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -443,18 +501,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -465,21 +511,39 @@
     <xf numFmtId="16" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -797,7 +861,7 @@
   <dimension ref="A1:Q35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -807,55 +871,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22">
+      <c r="B1" s="18">
         <v>43377</v>
       </c>
-      <c r="C1" s="22">
+      <c r="C1" s="18">
         <v>43384</v>
       </c>
-      <c r="D1" s="22">
+      <c r="D1" s="18">
         <v>43391</v>
       </c>
-      <c r="E1" s="23">
+      <c r="E1" s="19">
         <v>43398</v>
       </c>
-      <c r="F1" s="23">
+      <c r="F1" s="19">
         <v>43402</v>
       </c>
-      <c r="G1" s="23">
+      <c r="G1" s="19">
         <v>43412</v>
       </c>
-      <c r="H1" s="23">
+      <c r="H1" s="19">
         <v>43419</v>
       </c>
-      <c r="I1" s="23">
+      <c r="I1" s="19">
         <v>43426</v>
       </c>
-      <c r="J1" s="23">
+      <c r="J1" s="19">
         <v>43433</v>
       </c>
-      <c r="K1" s="23">
+      <c r="K1" s="19">
         <v>43440</v>
       </c>
-      <c r="L1" s="23">
+      <c r="L1" s="19">
         <v>43447</v>
       </c>
-      <c r="M1" s="23">
+      <c r="M1" s="19">
         <v>43454</v>
       </c>
-      <c r="N1" s="23">
+      <c r="N1" s="19">
         <v>43110</v>
       </c>
-      <c r="O1" s="23">
+      <c r="O1" s="19">
         <v>43117</v>
       </c>
-      <c r="P1" s="24">
+      <c r="P1" s="20">
         <v>43124</v>
       </c>
-      <c r="Q1" s="25" t="s">
+      <c r="Q1" s="21" t="s">
         <v>28</v>
       </c>
     </row>
@@ -865,7 +929,7 @@
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
-      <c r="D2" s="1"/>
+      <c r="D2" s="32"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -879,7 +943,7 @@
       <c r="O2" s="1"/>
       <c r="P2" s="15"/>
       <c r="Q2" s="16" t="str">
-        <f>LOOKUP((SUM(D2:O2)/SUM($D$18:$O$18))*10,$B$22:$B$27,$C$22:$C$27)</f>
+        <f>LOOKUP((SUM(D2:O2)/SUM($D$18:$O$18))*100,$B$22:$B$27,$C$22:$C$27)</f>
         <v>2.0</v>
       </c>
     </row>
@@ -889,7 +953,9 @@
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="1"/>
+      <c r="D3" s="3">
+        <v>2</v>
+      </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -903,7 +969,7 @@
       <c r="O3" s="1"/>
       <c r="P3" s="15"/>
       <c r="Q3" s="16" t="str">
-        <f t="shared" ref="Q3:Q16" si="0">LOOKUP((SUM(D3:O3)/SUM($D$18:$O$18))*10,$B$22:$B$27,$C$22:$C$27)</f>
+        <f>LOOKUP((SUM(D3:O3)/SUM($D$18:$O$18))*10,$B$22:$B$27,$C$22:$C$27)</f>
         <v>2.0</v>
       </c>
     </row>
@@ -913,7 +979,9 @@
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="1"/>
+      <c r="D4" s="3">
+        <v>2</v>
+      </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -927,7 +995,7 @@
       <c r="O4" s="1"/>
       <c r="P4" s="15"/>
       <c r="Q4" s="16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="Q3:Q7" si="0">LOOKUP((SUM(D4:O4)/SUM($D$18:$O$18))*10,$B$22:$B$27,$C$22:$C$27)</f>
         <v>2.0</v>
       </c>
     </row>
@@ -937,7 +1005,7 @@
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="1"/>
+      <c r="D5" s="3"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -961,7 +1029,7 @@
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="1"/>
+      <c r="D6" s="3"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -985,7 +1053,7 @@
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="1"/>
+      <c r="D7" s="4"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -1009,7 +1077,9 @@
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="1"/>
+      <c r="D8" s="3">
+        <v>2</v>
+      </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -1023,7 +1093,7 @@
       <c r="O8" s="1"/>
       <c r="P8" s="15"/>
       <c r="Q8" s="16" t="str">
-        <f t="shared" si="0"/>
+        <f>LOOKUP((SUM(D8:O8)/SUM($D$18:$O$18))*10,$B$22:$B$27,$C$22:$C$27)</f>
         <v>2.0</v>
       </c>
     </row>
@@ -1033,7 +1103,7 @@
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="1"/>
+      <c r="D9" s="3"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -1047,7 +1117,7 @@
       <c r="O9" s="1"/>
       <c r="P9" s="15"/>
       <c r="Q9" s="16" t="str">
-        <f t="shared" si="0"/>
+        <f>LOOKUP((SUM(D9:O9)/SUM($D$18:$O$18))*10,$B$22:$B$27,$C$22:$C$27)</f>
         <v>2.0</v>
       </c>
     </row>
@@ -1057,7 +1127,7 @@
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="1"/>
+      <c r="D10" s="3"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -1071,7 +1141,7 @@
       <c r="O10" s="1"/>
       <c r="P10" s="15"/>
       <c r="Q10" s="16" t="str">
-        <f t="shared" si="0"/>
+        <f>LOOKUP((SUM(D10:O10)/SUM($D$18:$O$18))*10,$B$22:$B$27,$C$22:$C$27)</f>
         <v>2.0</v>
       </c>
     </row>
@@ -1081,7 +1151,7 @@
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="1"/>
+      <c r="D11" s="3"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -1095,7 +1165,7 @@
       <c r="O11" s="1"/>
       <c r="P11" s="15"/>
       <c r="Q11" s="16" t="str">
-        <f t="shared" si="0"/>
+        <f>LOOKUP((SUM(D11:O11)/SUM($D$18:$O$18))*10,$B$22:$B$27,$C$22:$C$27)</f>
         <v>2.0</v>
       </c>
     </row>
@@ -1105,7 +1175,7 @@
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="1"/>
+      <c r="D12" s="3"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -1119,7 +1189,7 @@
       <c r="O12" s="1"/>
       <c r="P12" s="15"/>
       <c r="Q12" s="16" t="str">
-        <f t="shared" si="0"/>
+        <f>LOOKUP((SUM(D12:O12)/SUM($D$18:$O$18))*10,$B$22:$B$27,$C$22:$C$27)</f>
         <v>2.0</v>
       </c>
     </row>
@@ -1129,7 +1199,9 @@
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="1"/>
+      <c r="D13" s="3">
+        <v>2</v>
+      </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -1143,7 +1215,7 @@
       <c r="O13" s="1"/>
       <c r="P13" s="15"/>
       <c r="Q13" s="16" t="str">
-        <f t="shared" si="0"/>
+        <f>LOOKUP((SUM(D13:O13)/SUM($D$18:$O$18))*10,$B$22:$B$27,$C$22:$C$27)</f>
         <v>2.0</v>
       </c>
     </row>
@@ -1153,7 +1225,7 @@
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="1"/>
+      <c r="D14" s="3"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -1167,7 +1239,7 @@
       <c r="O14" s="1"/>
       <c r="P14" s="15"/>
       <c r="Q14" s="16" t="str">
-        <f t="shared" si="0"/>
+        <f>LOOKUP((SUM(D14:O14)/SUM($D$18:$O$18))*10,$B$22:$B$27,$C$22:$C$27)</f>
         <v>2.0</v>
       </c>
     </row>
@@ -1177,7 +1249,7 @@
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="1"/>
+      <c r="D15" s="3"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -1191,7 +1263,7 @@
       <c r="O15" s="1"/>
       <c r="P15" s="15"/>
       <c r="Q15" s="16" t="str">
-        <f t="shared" si="0"/>
+        <f>LOOKUP((SUM(D15:O15)/SUM($D$18:$O$18))*10,$B$22:$B$27,$C$22:$C$27)</f>
         <v>2.0</v>
       </c>
     </row>
@@ -1200,8 +1272,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="6"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3">
+        <v>2</v>
+      </c>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
@@ -1215,16 +1289,16 @@
       <c r="O16" s="6"/>
       <c r="P16" s="15"/>
       <c r="Q16" s="16" t="str">
-        <f t="shared" si="0"/>
+        <f>LOOKUP((SUM(D16:O16)/SUM($D$18:$O$18))*10,$B$22:$B$27,$C$22:$C$27)</f>
         <v>2.0</v>
       </c>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="20"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="29"/>
       <c r="D17" s="5" t="s">
         <v>16</v>
       </c>
@@ -1263,11 +1337,11 @@
       </c>
     </row>
     <row r="18" spans="1:15" ht="17" thickBot="1">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="18"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="27"/>
       <c r="D18" s="12">
         <v>10</v>
       </c>
@@ -1307,48 +1381,67 @@
     </row>
     <row r="20" spans="1:15" ht="17" thickBot="1"/>
     <row r="21" spans="1:15" ht="17" thickBot="1">
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="28"/>
+      <c r="C21" s="31"/>
+      <c r="E21" s="37" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="22" spans="1:15">
-      <c r="B22" s="30">
+      <c r="B22" s="24">
         <v>0</v>
       </c>
-      <c r="C22" s="31" t="s">
+      <c r="C22" s="25" t="s">
         <v>37</v>
+      </c>
+      <c r="E22" s="36"/>
+      <c r="F22" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:15">
       <c r="B23" s="9">
         <v>51</v>
       </c>
-      <c r="C23" s="29" t="s">
+      <c r="C23" s="23" t="s">
         <v>36</v>
+      </c>
+      <c r="E23" s="33"/>
+      <c r="F23" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:15">
       <c r="B24" s="9">
         <v>61</v>
       </c>
-      <c r="C24" s="29" t="s">
+      <c r="C24" s="23" t="s">
         <v>35</v>
+      </c>
+      <c r="E24" s="34"/>
+      <c r="F24" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:15">
       <c r="B25" s="9">
         <v>71</v>
       </c>
-      <c r="C25" s="29" t="s">
+      <c r="C25" s="23" t="s">
         <v>33</v>
+      </c>
+      <c r="E25" s="35"/>
+      <c r="F25" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:15">
       <c r="B26" s="9">
         <v>81</v>
       </c>
-      <c r="C26" s="29" t="s">
+      <c r="C26" s="23" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1356,33 +1449,33 @@
       <c r="B27" s="9">
         <v>91</v>
       </c>
-      <c r="C27" s="29" t="s">
+      <c r="C27" s="23" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:15">
-      <c r="C28" s="26"/>
+      <c r="C28" s="22"/>
     </row>
     <row r="29" spans="1:15">
-      <c r="C29" s="26"/>
+      <c r="C29" s="22"/>
     </row>
     <row r="30" spans="1:15">
-      <c r="C30" s="26"/>
+      <c r="C30" s="22"/>
     </row>
     <row r="31" spans="1:15">
-      <c r="C31" s="26"/>
+      <c r="C31" s="22"/>
     </row>
     <row r="32" spans="1:15">
-      <c r="C32" s="26"/>
+      <c r="C32" s="22"/>
     </row>
     <row r="33" spans="3:3">
-      <c r="C33" s="26"/>
+      <c r="C33" s="22"/>
     </row>
     <row r="34" spans="3:3">
-      <c r="C34" s="26"/>
+      <c r="C34" s="22"/>
     </row>
     <row r="35" spans="3:3">
-      <c r="C35" s="26"/>
+      <c r="C35" s="22"/>
     </row>
   </sheetData>
   <sortState ref="B22:C27">

</xml_diff>

<commit_message>
[assessment] update after 25.10.2018
</commit_message>
<xml_diff>
--- a/obecnosci_i_oceny.xlsx
+++ b/obecnosci_i_oceny.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neegra/paradygmaty-programowania/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AAEFD5E-1D16-664F-B6FC-8582C30B69B5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{690713BA-B6BD-A343-857E-BF2E36ED8CAA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="17100" xr2:uid="{97166A3A-37EA-D446-B119-A32076EDFA0A}"/>
   </bookViews>
@@ -866,7 +866,7 @@
   <dimension ref="A1:Q35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -935,7 +935,9 @@
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="35"/>
-      <c r="E2" s="1"/>
+      <c r="E2" s="32">
+        <v>1</v>
+      </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -959,9 +961,12 @@
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3">
+        <f>2+4</f>
+        <v>6</v>
+      </c>
+      <c r="E3" s="3">
         <v>2</v>
       </c>
-      <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -985,9 +990,12 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3">
+        <f>2+4</f>
+        <v>6</v>
+      </c>
+      <c r="E4" s="3">
         <v>2</v>
       </c>
-      <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -1010,8 +1018,10 @@
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="1"/>
+      <c r="D5" s="3">
+        <v>4</v>
+      </c>
+      <c r="E5" s="3"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -1034,8 +1044,12 @@
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="1"/>
+      <c r="D6" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="E6" s="32">
+        <v>1</v>
+      </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -1059,7 +1073,7 @@
       <c r="B7" s="4"/>
       <c r="C7" s="3"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="1"/>
+      <c r="E7" s="4"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -1083,9 +1097,11 @@
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3">
+        <v>6</v>
+      </c>
+      <c r="E8" s="3">
         <v>2</v>
       </c>
-      <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -1108,8 +1124,10 @@
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="1"/>
+      <c r="D9" s="3">
+        <v>2</v>
+      </c>
+      <c r="E9" s="3"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -1132,8 +1150,12 @@
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="1"/>
+      <c r="D10" s="3">
+        <v>5</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -1157,7 +1179,7 @@
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="1"/>
+      <c r="E11" s="4"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -1180,8 +1202,12 @@
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="1"/>
+      <c r="D12" s="3">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1</v>
+      </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -1205,9 +1231,11 @@
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3">
+        <v>6</v>
+      </c>
+      <c r="E13" s="3">
         <v>2</v>
       </c>
-      <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -1230,8 +1258,12 @@
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="1"/>
+      <c r="D14" s="3">
+        <v>4</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -1254,8 +1286,12 @@
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="1"/>
+      <c r="D15" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="E15" s="3">
+        <v>3</v>
+      </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -1279,9 +1315,9 @@
       <c r="B16" s="8"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3">
-        <v>2</v>
-      </c>
-      <c r="E16" s="6"/>
+        <v>5</v>
+      </c>
+      <c r="E16" s="32"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>

</xml_diff>

<commit_message>
[assessment] update after 29.10.2018
</commit_message>
<xml_diff>
--- a/obecnosci_i_oceny.xlsx
+++ b/obecnosci_i_oceny.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neegra/paradygmaty-programowania/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{690713BA-B6BD-A343-857E-BF2E36ED8CAA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E437B34A-BF37-AC44-82E7-AFDC2AE55055}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="17100" xr2:uid="{97166A3A-37EA-D446-B119-A32076EDFA0A}"/>
   </bookViews>
@@ -866,7 +866,7 @@
   <dimension ref="A1:Q35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -938,7 +938,9 @@
       <c r="E2" s="32">
         <v>1</v>
       </c>
-      <c r="F2" s="1"/>
+      <c r="F2" s="32">
+        <v>5</v>
+      </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -967,7 +969,9 @@
       <c r="E3" s="3">
         <v>2</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="F3" s="3">
+        <v>9</v>
+      </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -996,7 +1000,9 @@
       <c r="E4" s="3">
         <v>2</v>
       </c>
-      <c r="F4" s="1"/>
+      <c r="F4" s="3">
+        <v>6</v>
+      </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -1022,7 +1028,9 @@
         <v>4</v>
       </c>
       <c r="E5" s="3"/>
-      <c r="F5" s="1"/>
+      <c r="F5" s="3">
+        <v>3</v>
+      </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -1050,7 +1058,9 @@
       <c r="E6" s="32">
         <v>1</v>
       </c>
-      <c r="F6" s="1"/>
+      <c r="F6" s="3">
+        <v>3</v>
+      </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -1074,7 +1084,7 @@
       <c r="C7" s="3"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
-      <c r="F7" s="1"/>
+      <c r="F7" s="4"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -1102,7 +1112,9 @@
       <c r="E8" s="3">
         <v>2</v>
       </c>
-      <c r="F8" s="1"/>
+      <c r="F8" s="3">
+        <v>9</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -1128,7 +1140,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="3"/>
-      <c r="F9" s="1"/>
+      <c r="F9" s="3"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -1156,7 +1168,9 @@
       <c r="E10" s="3">
         <v>1</v>
       </c>
-      <c r="F10" s="1"/>
+      <c r="F10" s="3">
+        <v>6</v>
+      </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -1180,7 +1194,7 @@
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="1"/>
+      <c r="F11" s="4"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -1208,7 +1222,9 @@
       <c r="E12" s="3">
         <v>1</v>
       </c>
-      <c r="F12" s="1"/>
+      <c r="F12" s="3">
+        <v>5</v>
+      </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -1234,9 +1250,11 @@
         <v>6</v>
       </c>
       <c r="E13" s="3">
-        <v>2</v>
-      </c>
-      <c r="F13" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="F13" s="3">
+        <v>7</v>
+      </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -1264,7 +1282,9 @@
       <c r="E14" s="3">
         <v>1</v>
       </c>
-      <c r="F14" s="1"/>
+      <c r="F14" s="3">
+        <v>3</v>
+      </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -1292,7 +1312,9 @@
       <c r="E15" s="3">
         <v>3</v>
       </c>
-      <c r="F15" s="1"/>
+      <c r="F15" s="3">
+        <v>5</v>
+      </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -1318,7 +1340,9 @@
         <v>5</v>
       </c>
       <c r="E16" s="32"/>
-      <c r="F16" s="6"/>
+      <c r="F16" s="3">
+        <v>7</v>
+      </c>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>

</xml_diff>